<commit_message>
chỉnh sửa luồng đi
</commit_message>
<xml_diff>
--- a/Uploads/Book1.xlsx
+++ b/Uploads/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F214F0B-7953-4C96-840C-12DCD172EB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D83F70F-BFCD-4591-A17B-44A33E910470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{312F7849-C732-4D77-A136-BA2C873C6A55}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>EMAIL</t>
   </si>
@@ -118,9 +118,6 @@
     <t>duy.197pm21905@vanlanguni.vn</t>
   </si>
   <si>
-    <t>Đề tài 03: WEBSITE QUẢN LÝ TIẾN ĐỘ HỌC TẬP DÀNH CHO SINH VIÊN (Mức độ khó: Level 3)</t>
-  </si>
-  <si>
     <t>tuan.197pm31224@vanlanguni.vn</t>
   </si>
   <si>
@@ -154,17 +151,20 @@
     <t>Nguyễn Minh Tân</t>
   </si>
   <si>
-    <t>hiếu</t>
-  </si>
-  <si>
     <t>Trần Công Thanh</t>
+  </si>
+  <si>
+    <t>nguyen.197pm09482@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>lythihuyenchau@vanlanguni.vn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +200,15 @@
       <family val="1"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -398,10 +407,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -442,29 +452,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -777,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B10CCD1-A6C9-4FE1-A309-C960A450BB88}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -820,10 +834,10 @@
         <v>14</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -876,14 +890,14 @@
       <c r="B8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -891,7 +905,7 @@
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
     </row>
@@ -900,7 +914,7 @@
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
     </row>
@@ -909,7 +923,7 @@
       <c r="B11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
     </row>
@@ -918,7 +932,7 @@
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
     </row>
@@ -927,7 +941,7 @@
       <c r="B13" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="19"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
     </row>
@@ -938,20 +952,14 @@
       <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -960,7 +968,7 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -969,7 +977,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -978,49 +986,51 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8"/>
+      <c r="B20" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
         <v>4</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B21" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D21" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E21" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1029,7 +1039,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -1038,51 +1048,51 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
     </row>
-    <row r="25" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="15" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
         <v>5</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
+      <c r="D27" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -1091,7 +1101,7 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -1100,33 +1110,42 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="20"/>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
     </row>
+    <row r="32" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="D20:D25"/>
-    <mergeCell ref="D26:D31"/>
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="E20:E25"/>
-    <mergeCell ref="E26:E31"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="C21:C26"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="D14:D20"/>
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="E14:E20"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A27:A32"/>
     <mergeCell ref="C2:C7"/>
     <mergeCell ref="D2:D7"/>
     <mergeCell ref="E2:E7"/>
@@ -1136,6 +1155,10 @@
     <mergeCell ref="D8:D13"/>
     <mergeCell ref="E8:E13"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B20" r:id="rId1" xr:uid="{AD4EA750-30EB-4B4B-880D-434104535308}"/>
+    <hyperlink ref="B19" r:id="rId2" xr:uid="{DDA43518-4C3C-42C7-94A0-1A236143C0FF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code xong luồng đúng chức năng sprint 2
</commit_message>
<xml_diff>
--- a/Uploads/Book1.xlsx
+++ b/Uploads/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D83F70F-BFCD-4591-A17B-44A33E910470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FAE0E3-A1E7-4EA8-95B4-40D35A7C9826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{312F7849-C732-4D77-A136-BA2C873C6A55}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="122">
   <si>
     <t>EMAIL</t>
   </si>
@@ -157,14 +157,257 @@
     <t>nguyen.197pm09482@vanlanguni.vn</t>
   </si>
   <si>
-    <t>lythihuyenchau@vanlanguni.vn</t>
+    <t>tu.197pm33774@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>hoa.197pm09447@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>thai.197pm21979@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>toan.197pm09522@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>hau.197pm09444@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>dat.197pm31148@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>thanh.197pm31202@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>toan.197pm21992@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>thien.197pm21986@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>tuyen.197pm09538@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>luan.197pm09476@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>hau.197pm09443@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>huy.197pm09451@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>thang.197pm33773@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>linh.187pm06632@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>tuan.197pm21996@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>khuong.197pm09466@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>loc.197pm09474@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>hoang.197pm21928@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>tai.197pm21977@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>phu.197pm09495@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>ha.197pm09438@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>trung.197pm14606@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>dieu.197pm09425@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>nhan.197pm31185@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>triet.197pm31219@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>phu.197pm33529@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>duc.197pm34096@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>bao.197pm09417@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>tan.197ct22539@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>hiep.197pm31152@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>dung.197pm21901@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>nhi.197pm09485@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>danh.197pm21900@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>bao.197pm21896@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>cong.197pm21898@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>quang.197pm31194@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>dat.197pm09431@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>nam.197PM09478@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>dung.197pm31141@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>khoa.197pm31170@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>thang.197pm21984@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>thinh.197pm21988@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>lam.197lk21540@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>ngoc.197lh32654@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>long.197pm33931@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>tam.197pm34167@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>dai.197pm31146@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>tam.197pm31200@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>hung.187pm13922@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>an.197pm09415@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>khanh.197pm21938@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>tien.197pm09519@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>thang.197pm21981@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>quynh.197pm21974@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>hi.187pm23449@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>dat.197pm09434@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>minh.197pm31179@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>dat.197pm21912@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>long.197ct09826@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>vu.197pm31229@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>sang.187pm06699@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>Đề tài 03: WEBSITE QUẢN LÝ TIẾN ĐỘ HỌC TẬP DÀNH CHO SINH VIÊN (Mức độ khó: Level 3)</t>
+  </si>
+  <si>
+    <t>hiếu</t>
+  </si>
+  <si>
+    <t>Đề tài 06: WEBSITE VÀ ỨNG DỤNG ĐIỆN THOẠI QUẢN LÝ PHÍ (Mức độ khó: Level 3)</t>
+  </si>
+  <si>
+    <t>Đề tài 07: WEBSITE ĐĂNG KÝ XÉT TUYỂN HỌC BẠ (Mức độ khó: Level 3)</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Trung</t>
+  </si>
+  <si>
+    <t>Đề tài 08: WEBSITE ĐĂNG KÝ XÉT TUYỂN ĐGNL, THPT (Mức độ khó: Level 3)</t>
+  </si>
+  <si>
+    <t>Đề tài 09: WEBSITE XẾP PHÒNG CHO KHÁCH SẠN (Mức độ khó: Level 4)</t>
+  </si>
+  <si>
+    <t>Đặng Đình Hòa</t>
+  </si>
+  <si>
+    <t>Đề tài 10: ỨNG DỤNG VÍ ĐIỆN TỬ DÀNH CHO SINH VIÊN VĂN LANG  (Mức độ khó: Level 3)</t>
+  </si>
+  <si>
+    <t>Phạm Ngọc Duy</t>
+  </si>
+  <si>
+    <t>Đề tài 12: WEBSITE HỘP THƯ GÓP Ý DÀNH CHO SINH VIÊN KHOA CNTT (Mức độ khó: Level 2)</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Diễm Anh</t>
+  </si>
+  <si>
+    <t>Đề tài 13: ỨNG DỤNG HẸN HÒ Ở VĂN LANG (Mức độ khó: Level 3)</t>
+  </si>
+  <si>
+    <t>Đề tài 15: WEBSITE QUẢN LÝ MEETING (Mức độ khó: Level 2)</t>
+  </si>
+  <si>
+    <t>Lý Thị Huyền Châu</t>
+  </si>
+  <si>
+    <t>Đề tài 16: WEBSITE HOẶC ỨNG DỤNG ĐIỆN THOẠI QUẢN LÝ KINH DOANH CAFE (Mức độ khó: Level 3)</t>
+  </si>
+  <si>
+    <t>Phan Thị Hồng</t>
+  </si>
+  <si>
+    <t>Đề tài 17: WEBSITE CÂU LẠC BỘ VĂN LANG TECH (Mức độ khó: Level 3)</t>
+  </si>
+  <si>
+    <t>Đề tài 18: WEBSITE QUẢN LÝ DOANH NGHIỆP VINASA (Mức độ khó: Level 2)</t>
+  </si>
+  <si>
+    <t>Đề tài 19: WEBSITE QUẢN LÝ CÁC QUÁN ĂN XUNG QUANH TRƯỜNG VL (Mức độ khó: Level 3)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +462,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -240,7 +489,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -381,19 +630,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -411,7 +647,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -428,6 +664,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -437,27 +727,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -466,15 +735,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -791,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B10CCD1-A6C9-4FE1-A309-C960A450BB88}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -823,329 +1083,1036 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
       <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="14" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
         <v>2</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="15" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="24">
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="C14" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="14" t="s">
+      <c r="A17" s="25"/>
+      <c r="B17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="21" t="s">
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+    </row>
+    <row r="19" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="26"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="24">
+        <v>4</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+      <c r="B22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+    </row>
+    <row r="25" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="26"/>
+      <c r="B25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="24">
+        <v>5</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="25"/>
+      <c r="B28" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
+      <c r="B29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+    </row>
+    <row r="31" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="26"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="24">
+        <v>6</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="20" t="s">
+      <c r="C32" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="25"/>
+      <c r="B33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="25"/>
+      <c r="B34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="25"/>
+      <c r="B36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+    </row>
+    <row r="37" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="26"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="24">
+        <v>7</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="25"/>
+      <c r="B39" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="25"/>
+      <c r="B40" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="25"/>
+      <c r="B41" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="25"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+    </row>
+    <row r="43" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="26"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="24">
+        <v>8</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="25"/>
+      <c r="B45" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="25"/>
+      <c r="B46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="25"/>
+      <c r="B47" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="25"/>
+      <c r="B48" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+    </row>
+    <row r="49" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="26"/>
+      <c r="B49" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="24">
+        <v>9</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="25"/>
+      <c r="B51" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="25"/>
+      <c r="B52" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="25"/>
+      <c r="B53" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="25"/>
+      <c r="B54" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+    </row>
+    <row r="55" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="26"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="24">
+        <v>10</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="25"/>
+      <c r="B57" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="25"/>
+      <c r="B58" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="25"/>
+      <c r="B59" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="25"/>
+      <c r="B60" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+    </row>
+    <row r="61" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="26"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="24">
+        <v>11</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="25"/>
+      <c r="B63" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="25"/>
+      <c r="B64" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="25"/>
+      <c r="B65" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="25"/>
+      <c r="B66" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+    </row>
+    <row r="67" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="26"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="21">
+        <v>12</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="22"/>
+      <c r="B69" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="22"/>
+      <c r="B70" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="22"/>
+      <c r="B71" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="22"/>
+      <c r="B72" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C72" s="19"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+    </row>
+    <row r="73" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="23"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="22">
+        <v>13</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E74" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="22"/>
+      <c r="B75" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="22"/>
+      <c r="B76" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>4</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>5</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="19"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="22"/>
+      <c r="B77" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C77" s="19"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="19"/>
+    </row>
+    <row r="78" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="23"/>
+      <c r="B78" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C78" s="20"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="20"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="21">
+        <v>14</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E79" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="22"/>
+      <c r="B80" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="22"/>
+      <c r="B81" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C81" s="19"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="22"/>
+      <c r="B82" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="22"/>
+      <c r="B83" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C83" s="19"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+    </row>
+    <row r="84" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="23"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="20"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="21">
+        <v>15</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="22"/>
+      <c r="B86" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C86" s="19"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="19"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="22"/>
+      <c r="B87" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="22"/>
+      <c r="B88" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="22"/>
+      <c r="B89" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+    </row>
+    <row r="90" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="23"/>
+      <c r="B90" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C90" s="20"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="20"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="21">
+        <v>16</v>
+      </c>
+      <c r="B91" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E91" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="22"/>
+      <c r="B92" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="19"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="22"/>
+      <c r="B93" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C93" s="19"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="19"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="22"/>
+      <c r="B94" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C94" s="19"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="19"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="22"/>
+      <c r="B95" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C95" s="19"/>
+      <c r="D95" s="19"/>
+      <c r="E95" s="19"/>
+    </row>
+    <row r="96" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="23"/>
+      <c r="B96" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C96" s="20"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="20"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="21">
+        <v>17</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E97" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="22"/>
+      <c r="B98" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C98" s="19"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="19"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="22"/>
+      <c r="B99" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C99" s="19"/>
+      <c r="D99" s="19"/>
+      <c r="E99" s="19"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="22"/>
+      <c r="B100" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C100" s="19"/>
+      <c r="D100" s="19"/>
+      <c r="E100" s="19"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="22"/>
+      <c r="B101" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C101" s="19"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+    </row>
+    <row r="102" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="22"/>
+      <c r="B102" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C102" s="19"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="C21:C26"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="D14:D20"/>
-    <mergeCell ref="D21:D26"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="E14:E20"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A27:A32"/>
+  <mergeCells count="68">
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="C74:C78"/>
     <mergeCell ref="C2:C7"/>
     <mergeCell ref="D2:D7"/>
     <mergeCell ref="E2:E7"/>
@@ -1154,10 +2121,74 @@
     <mergeCell ref="C8:C13"/>
     <mergeCell ref="D8:D13"/>
     <mergeCell ref="E8:E13"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A50:A55"/>
+    <mergeCell ref="A56:A61"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="A68:A73"/>
+    <mergeCell ref="A74:A78"/>
+    <mergeCell ref="A79:A84"/>
+    <mergeCell ref="A85:A90"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="D26:D31"/>
+    <mergeCell ref="C32:C37"/>
+    <mergeCell ref="D32:D37"/>
+    <mergeCell ref="C38:C43"/>
+    <mergeCell ref="D38:D43"/>
+    <mergeCell ref="C44:C49"/>
+    <mergeCell ref="D44:D49"/>
+    <mergeCell ref="C50:C55"/>
+    <mergeCell ref="D50:D55"/>
+    <mergeCell ref="C56:C61"/>
+    <mergeCell ref="D56:D61"/>
+    <mergeCell ref="C62:C67"/>
+    <mergeCell ref="D62:D67"/>
+    <mergeCell ref="C68:C73"/>
+    <mergeCell ref="D68:D73"/>
+    <mergeCell ref="E79:E84"/>
+    <mergeCell ref="C79:C84"/>
+    <mergeCell ref="D79:D84"/>
+    <mergeCell ref="D74:D78"/>
+    <mergeCell ref="E74:E78"/>
+    <mergeCell ref="E44:E49"/>
+    <mergeCell ref="E50:E55"/>
+    <mergeCell ref="E56:E61"/>
+    <mergeCell ref="E62:E67"/>
+    <mergeCell ref="E68:E73"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="E20:E25"/>
+    <mergeCell ref="E26:E31"/>
+    <mergeCell ref="E32:E37"/>
+    <mergeCell ref="E38:E43"/>
+    <mergeCell ref="E85:E90"/>
+    <mergeCell ref="E91:E96"/>
+    <mergeCell ref="E97:E102"/>
+    <mergeCell ref="C91:C96"/>
+    <mergeCell ref="D91:D96"/>
+    <mergeCell ref="C97:C102"/>
+    <mergeCell ref="D97:D102"/>
+    <mergeCell ref="C85:C90"/>
+    <mergeCell ref="D85:D90"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B20" r:id="rId1" xr:uid="{AD4EA750-30EB-4B4B-880D-434104535308}"/>
-    <hyperlink ref="B19" r:id="rId2" xr:uid="{DDA43518-4C3C-42C7-94A0-1A236143C0FF}"/>
+    <hyperlink ref="B74" r:id="rId1" display="mailto:cong.197pm21898@vanlanguni.vn" xr:uid="{452CA6E2-FBFF-40E2-B5B3-0A86C52D7035}"/>
+    <hyperlink ref="B75" r:id="rId2" display="mailto:quang.197pm31194@vanlanguni.vn" xr:uid="{B9E376F9-FC66-4DF6-89A0-139777C46302}"/>
+    <hyperlink ref="B76" r:id="rId3" display="mailto:nguyen.197pm09482@vanlanguni.vn" xr:uid="{BAB61A2A-59A5-4454-ADAF-2B5580BFDAB0}"/>
+    <hyperlink ref="B77" r:id="rId4" display="mailto:dat.197pm09431@vanlanguni.vn" xr:uid="{6C89B2D4-D292-4475-ABCD-746A83E1942B}"/>
+    <hyperlink ref="B78" r:id="rId5" display="mailto:nam.197PM09478@vanlanguni.vn" xr:uid="{50449137-D486-49F4-9A94-06C829623501}"/>
+    <hyperlink ref="B91" r:id="rId6" display="mailto:an.197pm09415@vanlanguni.vn" xr:uid="{3E0FEE4E-828B-4902-A167-8E52B41F7678}"/>
+    <hyperlink ref="B92" r:id="rId7" display="mailto:khanh.197pm21938@vanlanguni.vn" xr:uid="{BFF097C6-CA06-490F-B922-8E4F29390199}"/>
+    <hyperlink ref="B93" r:id="rId8" display="mailto:tien.197pm09519@vanlanguni.vn" xr:uid="{A3387861-D2EF-465B-8B8A-BE9719C61FE3}"/>
+    <hyperlink ref="B94" r:id="rId9" display="mailto:thang.197pm21981@vanlanguni.vn" xr:uid="{B06CFECE-6A01-4FA0-A554-1592BA0BE3F3}"/>
+    <hyperlink ref="B95" r:id="rId10" display="mailto:quynh.197pm21974@vanlanguni.vn" xr:uid="{A4A8A437-1E7A-4AD9-80B6-4538AF44364F}"/>
+    <hyperlink ref="B96" r:id="rId11" display="mailto:hi.187pm23449@vanlanguni.vn" xr:uid="{F6502D0A-AEDD-4AEB-9BF3-B1AF7AE7BB1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>